<commit_message>
in order to merge from sebastian0 commits (#1)
* Mise à jour d'illustrations
Reprise du projet et isolation de l'erreur "segfault"

* Essai ajout illustration dans README.md

* Ajout illustration dans README.md

* Redimensionnement image README.md

* Correction merge
</commit_message>
<xml_diff>
--- a/RaF R-Pi.xlsx
+++ b/RaF R-Pi.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Suivit" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Suivit!$A$4:$J$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Suivit!$A$4:$J$38</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="62">
   <si>
     <t>Type</t>
   </si>
@@ -86,9 +86,6 @@
 http://raspberry-at-home.com/hotspot-wifi-access-point/
 En cas de problème :
 http://www.raspberrypi.org/forums/viewtopic.php?f=26&amp;t=49355</t>
-  </si>
-  <si>
-    <t>Instabilité du programme (Claix), utiliser Valgrind ou http://www.commentcamarche.net/faq/4791-langage-c-c-c-erreur-de-segmentation</t>
   </si>
   <si>
     <t>Date
@@ -310,6 +307,17 @@
   <si>
     <t>Générer la Documentation dans un format HTML.
 Modifier le contenu de fichiers doxygen ?!</t>
+  </si>
+  <si>
+    <t>Calculer le cout d'une journée
+PHT/kWh = 0.0892€  - Base, règlementé, 6kVA</t>
+  </si>
+  <si>
+    <t>Instabilité du programme (Claix), utiliser Valgrind ou http://www.commentcamarche.net/faq/4791-langage-c-c-c-erreur-de-segmentation
+=&gt; Erreur isolée, se produit lorsque ETX est avant STX</t>
+  </si>
+  <si>
+    <t>Rejeté</t>
   </si>
 </sst>
 </file>
@@ -810,7 +818,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J5" sqref="J5"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -867,35 +875,35 @@
         <v>0</v>
       </c>
       <c r="M1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="R1" s="10" t="s">
-        <v>49</v>
-      </c>
       <c r="S1" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="30">
       <c r="D2" s="15">
         <f>COUNTIF(G5:G59,D1)</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" s="16">
         <f>COUNTIF(G5:G59,E1)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2" s="15">
         <f>COUNTIF(G5:G59,F1)</f>
@@ -911,7 +919,7 @@
       </c>
       <c r="I2" s="17">
         <f>COUNTIF(D5:D59,"X")</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J2" s="17">
         <f>COUNTIF(E5:E59,"X")</f>
@@ -921,10 +929,10 @@
         <v>1</v>
       </c>
       <c r="M2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="N2" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>56</v>
       </c>
       <c r="O2" s="8"/>
       <c r="P2" s="8"/>
@@ -965,7 +973,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G4" s="9" t="s">
         <v>3</v>
@@ -977,7 +985,7 @@
         <v>8</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L4" s="13" t="s">
         <v>3</v>
@@ -991,20 +999,22 @@
       <c r="O4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="8"/>
+      <c r="P4" s="8" t="s">
+        <v>61</v>
+      </c>
       <c r="Q4" s="8"/>
       <c r="R4" s="8"/>
       <c r="S4" s="14"/>
     </row>
-    <row r="5" spans="1:19" ht="45">
+    <row r="5" spans="1:19" ht="60">
       <c r="A5" s="17">
         <v>11</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>13</v>
@@ -1016,10 +1026,10 @@
         <v>13</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="I5" s="19">
         <v>41766</v>
@@ -1031,10 +1041,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>12</v>
@@ -1049,7 +1059,7 @@
         <v>6</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I6" s="3">
         <v>41766</v>
@@ -1063,10 +1073,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>13</v>
@@ -1081,7 +1091,7 @@
         <v>5</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I7" s="19">
         <v>41334</v>
@@ -1093,10 +1103,10 @@
         <v>22</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>13</v>
@@ -1111,22 +1121,22 @@
         <v>4</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I8" s="19">
         <v>41782</v>
       </c>
       <c r="J8" s="15"/>
     </row>
-    <row r="9" spans="1:19" ht="30">
+    <row r="9" spans="1:19" ht="30" hidden="1">
       <c r="A9" s="17">
         <v>25</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>13</v>
@@ -1138,25 +1148,27 @@
         <v>13</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I9" s="19">
         <v>41874</v>
       </c>
-      <c r="J9" s="15"/>
+      <c r="J9" s="19">
+        <v>43412</v>
+      </c>
     </row>
     <row r="10" spans="1:19" ht="75">
       <c r="A10" s="17">
         <v>26</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>12</v>
@@ -1171,7 +1183,7 @@
         <v>4</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I10" s="19">
         <v>41883</v>
@@ -1183,10 +1195,10 @@
         <v>28</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>13</v>
@@ -1201,7 +1213,7 @@
         <v>4</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I11" s="19">
         <v>41906</v>
@@ -1213,10 +1225,10 @@
         <v>23</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>13</v>
@@ -1231,7 +1243,7 @@
         <v>4</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I12" s="20">
         <v>41782</v>
@@ -1243,10 +1255,10 @@
         <v>24</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>13</v>
@@ -1261,7 +1273,7 @@
         <v>4</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I13" s="20">
         <v>41782</v>
@@ -1273,10 +1285,10 @@
         <v>0</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>13</v>
@@ -1305,10 +1317,10 @@
         <v>1</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>12</v>
@@ -1323,7 +1335,7 @@
         <v>6</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I15" s="3">
         <v>41766</v>
@@ -1337,10 +1349,10 @@
         <v>7</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>13</v>
@@ -1367,10 +1379,10 @@
         <v>8</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>13</v>
@@ -1397,10 +1409,10 @@
         <v>29</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>13</v>
@@ -1415,7 +1427,7 @@
         <v>4</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I18" s="19">
         <v>41916</v>
@@ -1427,10 +1439,10 @@
         <v>32</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D19" s="15" t="s">
         <v>13</v>
@@ -1445,7 +1457,7 @@
         <v>4</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I19" s="19">
         <v>42121</v>
@@ -1457,10 +1469,10 @@
         <v>5</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>12</v>
@@ -1475,7 +1487,7 @@
         <v>6</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I20" s="3">
         <v>41766</v>
@@ -1489,10 +1501,10 @@
         <v>2</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>12</v>
@@ -1507,7 +1519,7 @@
         <v>6</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I21" s="3">
         <v>41766</v>
@@ -1521,10 +1533,10 @@
         <v>18</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>12</v>
@@ -1539,7 +1551,7 @@
         <v>6</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I22" s="3">
         <v>41768</v>
@@ -1553,10 +1565,10 @@
         <v>27</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>12</v>
@@ -1571,7 +1583,7 @@
         <v>6</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I23" s="3">
         <v>41904</v>
@@ -1583,10 +1595,10 @@
         <v>19</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>12</v>
@@ -1601,7 +1613,7 @@
         <v>6</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I24" s="3">
         <v>41768</v>
@@ -1610,15 +1622,15 @@
         <v>41904</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="17">
-        <v>6</v>
+    <row r="25" spans="1:10" ht="30">
+      <c r="A25" s="15">
+        <v>31</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D25" s="15" t="s">
         <v>12</v>
@@ -1632,29 +1644,29 @@
       <c r="G25" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="H25" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I25" s="19">
-        <v>41766</v>
-      </c>
-      <c r="J25" s="15"/>
+      <c r="H25" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I25" s="20">
+        <v>42699</v>
+      </c>
+      <c r="J25" s="8"/>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="17">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F26" s="15" t="s">
         <v>13</v>
@@ -1663,22 +1675,22 @@
         <v>4</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I26" s="19">
         <v>41766</v>
       </c>
       <c r="J26" s="15"/>
     </row>
-    <row r="27" spans="1:10" ht="60">
+    <row r="27" spans="1:10">
       <c r="A27" s="17">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D27" s="15" t="s">
         <v>13</v>
@@ -1693,10 +1705,10 @@
         <v>4</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I27" s="19">
-        <v>41768</v>
+        <v>41766</v>
       </c>
       <c r="J27" s="15"/>
     </row>
@@ -1705,10 +1717,10 @@
         <v>10</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>12</v>
@@ -1723,7 +1735,7 @@
         <v>6</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I28" s="3">
         <v>41766</v>
@@ -1737,10 +1749,10 @@
         <v>13</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>12</v>
@@ -1755,7 +1767,7 @@
         <v>6</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I29" s="3">
         <v>41766</v>
@@ -1769,10 +1781,10 @@
         <v>15</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>12</v>
@@ -1787,7 +1799,7 @@
         <v>6</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I30" s="3">
         <v>41766</v>
@@ -1796,12 +1808,12 @@
         <v>41904</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="30">
+    <row r="31" spans="1:10" ht="60">
       <c r="A31" s="17">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C31" s="15" t="s">
         <v>55</v>
@@ -1810,61 +1822,61 @@
         <v>13</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="G31" s="15" t="s">
         <v>4</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="I31" s="19">
+        <v>41768</v>
+      </c>
+      <c r="J31" s="15"/>
+    </row>
+    <row r="32" spans="1:10" ht="30">
+      <c r="A32" s="17">
+        <v>31</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G32" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I32" s="19">
         <v>42015</v>
       </c>
-      <c r="J31" s="15"/>
-    </row>
-    <row r="32" spans="1:10" ht="60">
-      <c r="A32" s="17">
-        <v>12</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E32" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G32" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="I32" s="19">
-        <v>41766</v>
-      </c>
       <c r="J32" s="15"/>
     </row>
-    <row r="33" spans="1:10" ht="30">
+    <row r="33" spans="1:10" ht="60">
       <c r="A33" s="17">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D33" s="15" t="s">
         <v>13</v>
@@ -1879,7 +1891,7 @@
         <v>5</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="I33" s="19">
         <v>41766</v>
@@ -1891,10 +1903,10 @@
         <v>16</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>13</v>
@@ -1909,7 +1921,7 @@
         <v>6</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I34" s="3">
         <v>41766</v>
@@ -1923,10 +1935,10 @@
         <v>20</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>13</v>
@@ -1941,7 +1953,7 @@
         <v>6</v>
       </c>
       <c r="H35" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I35" s="3">
         <v>41768</v>
@@ -1952,31 +1964,31 @@
     </row>
     <row r="36" spans="1:10" ht="30">
       <c r="A36" s="17">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F36" s="15" t="s">
         <v>13</v>
       </c>
       <c r="G36" s="15" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="I36" s="19">
-        <v>41917</v>
+        <v>41766</v>
       </c>
       <c r="J36" s="15"/>
     </row>
@@ -1985,10 +1997,10 @@
         <v>17</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2" t="s">
@@ -2001,7 +2013,7 @@
         <v>6</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I37" s="3">
         <v>41766</v>
@@ -2010,17 +2022,35 @@
         <v>42121</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
-      <c r="A38" s="15"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
+    <row r="38" spans="1:10" ht="30">
+      <c r="A38" s="17">
+        <v>30</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I38" s="19">
+        <v>41917</v>
+      </c>
+      <c r="J38" s="15"/>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="15"/>
@@ -2275,7 +2305,7 @@
       <c r="J59" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:J37">
+  <autoFilter ref="A4:J38">
     <filterColumn colId="5"/>
     <filterColumn colId="6">
       <filters>
@@ -2283,10 +2313,6 @@
         <filter val="Ouvert"/>
       </filters>
     </filterColumn>
-    <sortState ref="A5:J37">
-      <sortCondition ref="B5:B37"/>
-      <sortCondition ref="C5:C37"/>
-    </sortState>
   </autoFilter>
   <sortState ref="A3:I20">
     <sortCondition ref="E3:E20"/>
@@ -2314,7 +2340,7 @@
       <formula1>$M$3:$N$3</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Statut" sqref="G5:G59">
-      <formula1>$M$4:$O$4</formula1>
+      <formula1>$M$4:$P$4</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Revert "in order to merge from sebastian0 commits (#1)"
This reverts commit fb584944cf8e4d3c031c2a0c14c3c69866cf1018.
</commit_message>
<xml_diff>
--- a/RaF R-Pi.xlsx
+++ b/RaF R-Pi.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Suivit" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Suivit!$A$4:$J$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Suivit!$A$4:$J$37</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="60">
   <si>
     <t>Type</t>
   </si>
@@ -86,6 +86,9 @@
 http://raspberry-at-home.com/hotspot-wifi-access-point/
 En cas de problème :
 http://www.raspberrypi.org/forums/viewtopic.php?f=26&amp;t=49355</t>
+  </si>
+  <si>
+    <t>Instabilité du programme (Claix), utiliser Valgrind ou http://www.commentcamarche.net/faq/4791-langage-c-c-c-erreur-de-segmentation</t>
   </si>
   <si>
     <t>Date
@@ -307,17 +310,6 @@
   <si>
     <t>Générer la Documentation dans un format HTML.
 Modifier le contenu de fichiers doxygen ?!</t>
-  </si>
-  <si>
-    <t>Calculer le cout d'une journée
-PHT/kWh = 0.0892€  - Base, règlementé, 6kVA</t>
-  </si>
-  <si>
-    <t>Instabilité du programme (Claix), utiliser Valgrind ou http://www.commentcamarche.net/faq/4791-langage-c-c-c-erreur-de-segmentation
-=&gt; Erreur isolée, se produit lorsque ETX est avant STX</t>
-  </si>
-  <si>
-    <t>Rejeté</t>
   </si>
 </sst>
 </file>
@@ -818,7 +810,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -875,35 +867,35 @@
         <v>0</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="P1" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Q1" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="R1" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="S1" s="21" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="30">
       <c r="D2" s="15">
         <f>COUNTIF(G5:G59,D1)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" s="16">
         <f>COUNTIF(G5:G59,E1)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" s="15">
         <f>COUNTIF(G5:G59,F1)</f>
@@ -919,7 +911,7 @@
       </c>
       <c r="I2" s="17">
         <f>COUNTIF(D5:D59,"X")</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J2" s="17">
         <f>COUNTIF(E5:E59,"X")</f>
@@ -929,10 +921,10 @@
         <v>1</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="O2" s="8"/>
       <c r="P2" s="8"/>
@@ -973,7 +965,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G4" s="9" t="s">
         <v>3</v>
@@ -985,7 +977,7 @@
         <v>8</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L4" s="13" t="s">
         <v>3</v>
@@ -999,22 +991,20 @@
       <c r="O4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="8" t="s">
-        <v>61</v>
-      </c>
+      <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
       <c r="R4" s="8"/>
       <c r="S4" s="14"/>
     </row>
-    <row r="5" spans="1:19" ht="60">
+    <row r="5" spans="1:19" ht="45">
       <c r="A5" s="17">
         <v>11</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>13</v>
@@ -1026,10 +1016,10 @@
         <v>13</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="I5" s="19">
         <v>41766</v>
@@ -1041,10 +1031,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>12</v>
@@ -1059,7 +1049,7 @@
         <v>6</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I6" s="3">
         <v>41766</v>
@@ -1073,10 +1063,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>13</v>
@@ -1091,7 +1081,7 @@
         <v>5</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I7" s="19">
         <v>41334</v>
@@ -1103,10 +1093,10 @@
         <v>22</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>13</v>
@@ -1121,22 +1111,22 @@
         <v>4</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I8" s="19">
         <v>41782</v>
       </c>
       <c r="J8" s="15"/>
     </row>
-    <row r="9" spans="1:19" ht="30" hidden="1">
+    <row r="9" spans="1:19" ht="30">
       <c r="A9" s="17">
         <v>25</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>13</v>
@@ -1148,27 +1138,25 @@
         <v>13</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>61</v>
+        <v>4</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I9" s="19">
         <v>41874</v>
       </c>
-      <c r="J9" s="19">
-        <v>43412</v>
-      </c>
+      <c r="J9" s="15"/>
     </row>
     <row r="10" spans="1:19" ht="75">
       <c r="A10" s="17">
         <v>26</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>12</v>
@@ -1183,7 +1171,7 @@
         <v>4</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I10" s="19">
         <v>41883</v>
@@ -1195,10 +1183,10 @@
         <v>28</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>13</v>
@@ -1213,7 +1201,7 @@
         <v>4</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I11" s="19">
         <v>41906</v>
@@ -1225,10 +1213,10 @@
         <v>23</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>13</v>
@@ -1243,7 +1231,7 @@
         <v>4</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I12" s="20">
         <v>41782</v>
@@ -1255,10 +1243,10 @@
         <v>24</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>13</v>
@@ -1273,7 +1261,7 @@
         <v>4</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I13" s="20">
         <v>41782</v>
@@ -1285,10 +1273,10 @@
         <v>0</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>13</v>
@@ -1317,10 +1305,10 @@
         <v>1</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>12</v>
@@ -1335,7 +1323,7 @@
         <v>6</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I15" s="3">
         <v>41766</v>
@@ -1349,10 +1337,10 @@
         <v>7</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>13</v>
@@ -1379,10 +1367,10 @@
         <v>8</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>13</v>
@@ -1409,10 +1397,10 @@
         <v>29</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>13</v>
@@ -1427,7 +1415,7 @@
         <v>4</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I18" s="19">
         <v>41916</v>
@@ -1439,10 +1427,10 @@
         <v>32</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D19" s="15" t="s">
         <v>13</v>
@@ -1457,7 +1445,7 @@
         <v>4</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I19" s="19">
         <v>42121</v>
@@ -1469,10 +1457,10 @@
         <v>5</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>12</v>
@@ -1487,7 +1475,7 @@
         <v>6</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I20" s="3">
         <v>41766</v>
@@ -1501,10 +1489,10 @@
         <v>2</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>12</v>
@@ -1519,7 +1507,7 @@
         <v>6</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I21" s="3">
         <v>41766</v>
@@ -1533,10 +1521,10 @@
         <v>18</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>12</v>
@@ -1551,7 +1539,7 @@
         <v>6</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I22" s="3">
         <v>41768</v>
@@ -1565,10 +1553,10 @@
         <v>27</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>12</v>
@@ -1583,7 +1571,7 @@
         <v>6</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I23" s="3">
         <v>41904</v>
@@ -1595,10 +1583,10 @@
         <v>19</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>12</v>
@@ -1613,7 +1601,7 @@
         <v>6</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I24" s="3">
         <v>41768</v>
@@ -1622,15 +1610,15 @@
         <v>41904</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="30">
-      <c r="A25" s="15">
-        <v>31</v>
+    <row r="25" spans="1:10">
+      <c r="A25" s="17">
+        <v>6</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D25" s="15" t="s">
         <v>12</v>
@@ -1644,29 +1632,29 @@
       <c r="G25" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="H25" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="I25" s="20">
-        <v>42699</v>
-      </c>
-      <c r="J25" s="8"/>
+      <c r="H25" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I25" s="19">
+        <v>41766</v>
+      </c>
+      <c r="J25" s="15"/>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="17">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F26" s="15" t="s">
         <v>13</v>
@@ -1675,22 +1663,22 @@
         <v>4</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I26" s="19">
         <v>41766</v>
       </c>
       <c r="J26" s="15"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" ht="60">
       <c r="A27" s="17">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D27" s="15" t="s">
         <v>13</v>
@@ -1705,10 +1693,10 @@
         <v>4</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I27" s="19">
-        <v>41766</v>
+        <v>41768</v>
       </c>
       <c r="J27" s="15"/>
     </row>
@@ -1717,10 +1705,10 @@
         <v>10</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>12</v>
@@ -1735,7 +1723,7 @@
         <v>6</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I28" s="3">
         <v>41766</v>
@@ -1749,10 +1737,10 @@
         <v>13</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>12</v>
@@ -1767,7 +1755,7 @@
         <v>6</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I29" s="3">
         <v>41766</v>
@@ -1781,10 +1769,10 @@
         <v>15</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>12</v>
@@ -1799,7 +1787,7 @@
         <v>6</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I30" s="3">
         <v>41766</v>
@@ -1808,12 +1796,12 @@
         <v>41904</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="60">
+    <row r="31" spans="1:10" ht="30">
       <c r="A31" s="17">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C31" s="15" t="s">
         <v>55</v>
@@ -1822,61 +1810,61 @@
         <v>13</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="G31" s="15" t="s">
         <v>4</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="I31" s="19">
-        <v>41768</v>
+        <v>42015</v>
       </c>
       <c r="J31" s="15"/>
     </row>
-    <row r="32" spans="1:10" ht="30">
+    <row r="32" spans="1:10" ht="60">
       <c r="A32" s="17">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D32" s="15" t="s">
         <v>13</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="G32" s="15" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="I32" s="19">
-        <v>42015</v>
+        <v>41766</v>
       </c>
       <c r="J32" s="15"/>
     </row>
-    <row r="33" spans="1:10" ht="60">
+    <row r="33" spans="1:10" ht="30">
       <c r="A33" s="17">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D33" s="15" t="s">
         <v>13</v>
@@ -1891,7 +1879,7 @@
         <v>5</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="I33" s="19">
         <v>41766</v>
@@ -1903,10 +1891,10 @@
         <v>16</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>13</v>
@@ -1921,7 +1909,7 @@
         <v>6</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I34" s="3">
         <v>41766</v>
@@ -1935,10 +1923,10 @@
         <v>20</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>13</v>
@@ -1953,7 +1941,7 @@
         <v>6</v>
       </c>
       <c r="H35" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I35" s="3">
         <v>41768</v>
@@ -1964,31 +1952,31 @@
     </row>
     <row r="36" spans="1:10" ht="30">
       <c r="A36" s="17">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F36" s="15" t="s">
         <v>13</v>
       </c>
       <c r="G36" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="I36" s="19">
-        <v>41766</v>
+        <v>41917</v>
       </c>
       <c r="J36" s="15"/>
     </row>
@@ -1997,10 +1985,10 @@
         <v>17</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2" t="s">
@@ -2013,7 +2001,7 @@
         <v>6</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I37" s="3">
         <v>41766</v>
@@ -2022,35 +2010,17 @@
         <v>42121</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="30">
-      <c r="A38" s="17">
-        <v>30</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="D38" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E38" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F38" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G38" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="H38" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="I38" s="19">
-        <v>41917</v>
-      </c>
-      <c r="J38" s="15"/>
+    <row r="38" spans="1:10">
+      <c r="A38" s="15"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="15"/>
@@ -2305,7 +2275,7 @@
       <c r="J59" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:J38">
+  <autoFilter ref="A4:J37">
     <filterColumn colId="5"/>
     <filterColumn colId="6">
       <filters>
@@ -2313,6 +2283,10 @@
         <filter val="Ouvert"/>
       </filters>
     </filterColumn>
+    <sortState ref="A5:J37">
+      <sortCondition ref="B5:B37"/>
+      <sortCondition ref="C5:C37"/>
+    </sortState>
   </autoFilter>
   <sortState ref="A3:I20">
     <sortCondition ref="E3:E20"/>
@@ -2340,7 +2314,7 @@
       <formula1>$M$3:$N$3</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Statut" sqref="G5:G59">
-      <formula1>$M$4:$P$4</formula1>
+      <formula1>$M$4:$O$4</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>